<commit_message>
Gráficos de dificuldades no uso de mídias sociais para educação gerado.
</commit_message>
<xml_diff>
--- a/dados/umses_alunos_2018.xlsx
+++ b/dados/umses_alunos_2018.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb95d6a7f4534cf5/Projetos 2018/Ciencia de Dados/Introducao a Ciencia de Dados/Trabalhos 2018/Questionario/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Important stuff\UNESP\3o Ano - 2o Semestre\Data Science\Trabalho final\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4A67720-6036-4B94-87F7-0E048FFD3453}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CF1709-ACCE-4E9B-A247-C05B8535C287}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5580" xr2:uid="{D5DFAED4-3D0B-4958-B9A2-2717804177B8}"/>
   </bookViews>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C17B252-379D-4503-BCAA-F6A83E41DDC2}">
   <dimension ref="A1:AR69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="S38" workbookViewId="0">
+      <selection activeCell="AL52" sqref="AL52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5243,9 +5243,6 @@
       <c r="AF50">
         <v>3</v>
       </c>
-      <c r="AL50" t="s">
-        <v>53</v>
-      </c>
       <c r="AM50">
         <v>1</v>
       </c>
@@ -5329,6 +5326,9 @@
       <c r="AI51">
         <v>1</v>
       </c>
+      <c r="AL51" t="s">
+        <v>53</v>
+      </c>
       <c r="AM51">
         <v>1</v>
       </c>
@@ -6955,5 +6955,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>